<commit_message>
Actualizacion DAS y planilla de requerimientos (ajustes fase 2)
</commit_message>
<xml_diff>
--- a/FASE 2/Evidencias Proyecto/Evidencias de Documentacion/Planilla de requerimientos.xlsx
+++ b/FASE 2/Evidencias Proyecto/Evidencias de Documentacion/Planilla de requerimientos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duoc\Capstone\Evaluacion Fase 2\Completanding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C9B00E-A4B0-4A43-B890-6A10C2BA2BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53FEA92-5FC7-45CA-8F71-081E34A2FA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
   <si>
     <t>[R-N°]</t>
   </si>
@@ -80,9 +80,6 @@
     <t>RNF-01</t>
   </si>
   <si>
-    <t>Fiabilidad Clínica (Sensibilidad)</t>
-  </si>
-  <si>
     <t>No Funcional</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>RNF-05</t>
   </si>
   <si>
-    <t>Seguridad de Datos</t>
-  </si>
-  <si>
     <t>Entradas</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t>30 parámetros morfológicos (Radio, Textura, Perímetro, etc.)</t>
   </si>
   <si>
-    <t>1. Validación de rangos numéricos.    2. Ejecución de modelo (RF/SVM).</t>
-  </si>
-  <si>
     <t>Etiqueta de clase: Maligno (1) o Benigno (0) con % de probabilidad.</t>
   </si>
   <si>
@@ -143,18 +134,6 @@
     <t>Tablero interactivo con métricas de Recall y distribución de casos.</t>
   </si>
   <si>
-    <t>Conexión a internet estable y cuenta de Power BI activa.</t>
-  </si>
-  <si>
-    <t>Criterios de filtro (Fecha, ID Paciente, Tipo Diagnóstico).</t>
-  </si>
-  <si>
-    <t>Búsqueda y filtrado en la base de datos local (Dataframe).</t>
-  </si>
-  <si>
-    <t>Lista de registros que coinciden con la búsqueda.</t>
-  </si>
-  <si>
     <t>Existencia de registros previos en el historial.</t>
   </si>
   <si>
@@ -164,9 +143,6 @@
     <t>Criterio de aceptación (Métrica)</t>
   </si>
   <si>
-    <t>Fiabilidad Clínica</t>
-  </si>
-  <si>
     <t>Calidad / Fiabilidad</t>
   </si>
   <si>
@@ -179,9 +155,6 @@
     <t>Rendimiento</t>
   </si>
   <si>
-    <t>El tiempo de respuesta del motor de ML no debe interrumpir el flujo de la consulta médica.</t>
-  </si>
-  <si>
     <t>Tiempo de procesamiento &lt; 3 segundos tras envío.</t>
   </si>
   <si>
@@ -197,19 +170,43 @@
     <t>Disponibilidad</t>
   </si>
   <si>
-    <t>La herramienta debe estar accesible durante el horario de atención médica estándar.</t>
-  </si>
-  <si>
-    <t>Disponibilidad &gt; 99% (SLA Google Cloud).</t>
-  </si>
-  <si>
     <t>Seguridad</t>
   </si>
   <si>
-    <t>Los datos procesados no deben ser accesibles públicamente fuera del entorno clínico.</t>
-  </si>
-  <si>
-    <t>Acceso restringido mediante credenciales de Google.</t>
+    <t>Criterios de filtro (Fecha, ID de Predicción/Registro, Resultado: Benigno/Maligno).</t>
+  </si>
+  <si>
+    <t>Búsqueda y filtrado sobre el historial de predicciones almacenado (CSV/Excel o estructura local generada por el prototipo).</t>
+  </si>
+  <si>
+    <t>Lista de predicciones que coinciden con los criterios (sin PII).</t>
+  </si>
+  <si>
+    <t>Existe archivo fuente (CSV/Excel) de historial y Power BI está configurado para leerlo (refresh manual o programado según entorno).</t>
+  </si>
+  <si>
+    <t>La disponibilidad depende de servicios externos (Drive/Colab/Power BI). Para fines académicos se requiere disponibilidad suficiente durante sesiones de trabajo, sin SLA garantizado.</t>
+  </si>
+  <si>
+    <t>Disponibilidad operativa: acceso exitoso a la solución en &gt; 9 de 10 intentos durante la ventana de pruebas (sin SLA).</t>
+  </si>
+  <si>
+    <t>Los archivos del proyecto (dataset público y el historial de predicciones) deben mantenerse sin datos personales identificables (sin PII) y con acceso restringido.</t>
+  </si>
+  <si>
+    <t>Permisos “Restringido” en Drive/local (solo autora/docente) y el historial no incluye PII (sin nombre, RUT, ID paciente).</t>
+  </si>
+  <si>
+    <t>Seguridad y privacidad (sin PII)</t>
+  </si>
+  <si>
+    <t>Ejecución del modelo seleccionado (RF/SVM/RL) para inferencia.</t>
+  </si>
+  <si>
+    <t>El tiempo de respuesta del motor de ML no debe interrumpir el flujo de uso del prototipo.</t>
+  </si>
+  <si>
+    <t>Fiabilidad Clínica (Recall)</t>
   </si>
 </sst>
 </file>
@@ -605,7 +602,7 @@
   <dimension ref="A1:F997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -694,10 +691,10 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -709,13 +706,13 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -727,13 +724,13 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -745,13 +742,13 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -762,13 +759,13 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -1802,7 +1799,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1810,7 +1807,7 @@
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="36.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
@@ -1826,10 +1823,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -1842,84 +1839,84 @@
         <v>16</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>20</v>
-      </c>
       <c r="C3" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="B5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="E5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="16" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="E6" s="16" t="s">
         <v>55</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2929,7 +2926,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2949,16 +2946,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2969,19 +2966,19 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -2989,19 +2986,19 @@
         <v>11</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
@@ -3009,16 +3006,16 @@
         <v>14</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>